<commit_message>
Menghilangkan space di akhir age 0-4 supaya bisa terdeteksi regex pada usia
</commit_message>
<xml_diff>
--- a/public/Tabel Premi.xlsx
+++ b/public/Tabel Premi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aldal\ivanmsig\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2D4012-EA6C-4DC6-BC5D-7EA59A38F60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860DB8C0-684C-4CE2-A28E-A9E872AEFC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{363548B0-63E0-5348-93B9-9279F5F3BE45}"/>
   </bookViews>
@@ -28,9 +28,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="32">
   <si>
-    <t xml:space="preserve">0-4 </t>
-  </si>
-  <si>
     <t>usia (tahun)</t>
   </si>
   <si>
@@ -122,6 +119,9 @@
   </si>
   <si>
     <t>Harga / tahun</t>
+  </si>
+  <si>
+    <t>0-4</t>
   </si>
 </sst>
 </file>
@@ -131,7 +131,7 @@
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -142,6 +142,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -184,19 +190,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -516,8 +522,8 @@
   <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K47" sqref="K47"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -530,1009 +536,1009 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8"/>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.6">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="7" t="s">
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="2" t="s">
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="6"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A3" s="9" t="s">
-        <v>0</v>
+      <c r="A3" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="B3" s="1">
         <v>4907000</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A4" s="9" t="s">
-        <v>0</v>
+      <c r="A4" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="B4" s="1">
         <v>6282000</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A5" s="9" t="s">
-        <v>0</v>
+      <c r="A5" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="B5" s="1">
         <v>7558000</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A6" s="9" t="s">
-        <v>0</v>
+      <c r="A6" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="B6" s="1">
         <v>11488000</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
         <v>19</v>
       </c>
-      <c r="I6" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A7" s="10" t="s">
-        <v>18</v>
+      <c r="A7" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="B7" s="1">
         <v>4383000</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A8" s="10" t="s">
-        <v>18</v>
+      <c r="A8" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="B8" s="1">
         <v>5631000</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A9" s="10" t="s">
-        <v>18</v>
+      <c r="A9" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="B9" s="1">
         <v>6873000</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A10" s="10" t="s">
-        <v>18</v>
+      <c r="A10" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="B10" s="1">
         <v>10592000</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" t="s">
         <v>19</v>
       </c>
-      <c r="I10" t="s">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.6">
+      <c r="A11" s="6" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A11" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="B11" s="1">
         <v>4904000</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A12" s="9" t="s">
-        <v>21</v>
+      <c r="A12" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="B12" s="1">
         <v>6210000</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A13" s="9" t="s">
-        <v>21</v>
+      <c r="A13" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="B13" s="1">
         <v>7639000</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A14" s="9" t="s">
-        <v>21</v>
+      <c r="A14" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="B14" s="1">
         <v>11679000</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" t="s">
         <v>19</v>
       </c>
-      <c r="I14" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A15" s="9" t="s">
-        <v>22</v>
+      <c r="A15" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B15" s="1">
         <v>5528000</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A16" s="9" t="s">
-        <v>22</v>
+      <c r="A16" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B16" s="1">
         <v>6956000</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A17" s="9" t="s">
-        <v>22</v>
+      <c r="A17" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B17" s="1">
         <v>8303000</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A18" s="9" t="s">
-        <v>22</v>
+      <c r="A18" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B18" s="1">
         <v>12928000</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H18" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" t="s">
         <v>19</v>
       </c>
-      <c r="I18" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A19" s="9" t="s">
-        <v>23</v>
+      <c r="A19" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="B19" s="1">
         <v>6212000</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A20" s="9" t="s">
-        <v>23</v>
+      <c r="A20" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="B20" s="1">
         <v>7898000</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A21" s="9" t="s">
-        <v>23</v>
+      <c r="A21" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="B21" s="1">
         <v>9109000</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A22" s="9" t="s">
-        <v>23</v>
+      <c r="A22" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="B22" s="1">
         <v>14406000</v>
       </c>
       <c r="E22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" t="s">
         <v>19</v>
       </c>
-      <c r="I22" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A23" s="9" t="s">
-        <v>24</v>
+      <c r="A23" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="B23" s="1">
         <v>6863000</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A24" s="9" t="s">
-        <v>24</v>
+      <c r="A24" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="B24" s="1">
         <v>9429000</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A25" s="9" t="s">
-        <v>24</v>
+      <c r="A25" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="B25" s="1">
         <v>10875000</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A26" s="9" t="s">
-        <v>24</v>
+      <c r="A26" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="B26" s="1">
         <v>17323000</v>
       </c>
       <c r="E26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H26" t="s">
+        <v>18</v>
+      </c>
+      <c r="I26" t="s">
         <v>19</v>
       </c>
-      <c r="I26" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A27" s="9" t="s">
-        <v>25</v>
+      <c r="A27" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="B27" s="1">
         <v>8751000</v>
       </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A28" s="9" t="s">
-        <v>25</v>
+      <c r="A28" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="B28" s="1">
         <v>11894000</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A29" s="9" t="s">
-        <v>25</v>
+      <c r="A29" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="B29" s="1">
         <v>14219000</v>
       </c>
       <c r="D29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A30" s="9" t="s">
-        <v>25</v>
+      <c r="A30" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="B30" s="1">
         <v>20805000</v>
       </c>
       <c r="E30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H30" t="s">
+        <v>18</v>
+      </c>
+      <c r="I30" t="s">
         <v>19</v>
       </c>
-      <c r="I30" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A31" s="9" t="s">
-        <v>26</v>
+      <c r="A31" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="B31" s="1">
         <v>11649000</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A32" s="9" t="s">
-        <v>26</v>
+      <c r="A32" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="B32" s="1">
         <v>15861000</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A33" s="9" t="s">
-        <v>26</v>
+      <c r="A33" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="B33" s="1">
         <v>17504000</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A34" s="9" t="s">
-        <v>26</v>
+      <c r="A34" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="B34" s="1">
         <v>26260000</v>
       </c>
       <c r="E34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H34" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" t="s">
         <v>19</v>
       </c>
-      <c r="I34" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A35" s="9" t="s">
-        <v>27</v>
+      <c r="A35" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="B35" s="1">
         <v>16505000</v>
       </c>
       <c r="C35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A36" s="9" t="s">
-        <v>27</v>
+      <c r="A36" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="B36" s="1">
         <v>21909000</v>
       </c>
       <c r="C36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A37" s="9" t="s">
-        <v>27</v>
+      <c r="A37" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="B37" s="1">
         <v>23497000</v>
       </c>
       <c r="D37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A38" s="9" t="s">
-        <v>27</v>
+      <c r="A38" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="B38" s="1">
         <v>38844000</v>
       </c>
       <c r="E38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H38" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" t="s">
         <v>19</v>
       </c>
-      <c r="I38" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A39" s="9" t="s">
-        <v>28</v>
+      <c r="A39" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="B39" s="1">
         <v>19826000</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A40" s="9" t="s">
-        <v>28</v>
+      <c r="A40" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="B40" s="1">
         <v>25670000</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A41" s="9" t="s">
-        <v>28</v>
+      <c r="A41" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="B41" s="1">
         <v>27950000</v>
       </c>
       <c r="D41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A42" s="9" t="s">
-        <v>28</v>
+      <c r="A42" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="B42" s="1">
         <v>39451000</v>
       </c>
       <c r="E42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H42" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" t="s">
         <v>19</v>
       </c>
-      <c r="I42" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A43" s="9" t="s">
-        <v>29</v>
+      <c r="A43" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="B43" s="1">
         <v>25970000</v>
       </c>
       <c r="C43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H43" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A44" s="9" t="s">
-        <v>29</v>
+      <c r="A44" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="B44" s="1">
         <v>34526000</v>
       </c>
       <c r="C44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A45" s="9" t="s">
-        <v>29</v>
+      <c r="A45" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="B45" s="1">
         <v>38848000</v>
       </c>
       <c r="D45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A46" s="9" t="s">
-        <v>29</v>
+      <c r="A46" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="B46" s="1">
         <v>56804000</v>
       </c>
       <c r="E46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H46" t="s">
+        <v>18</v>
+      </c>
+      <c r="I46" t="s">
         <v>19</v>
       </c>
-      <c r="I46" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A47" s="9" t="s">
-        <v>30</v>
+      <c r="A47" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="B47" s="1">
         <v>33534000</v>
       </c>
       <c r="C47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H47" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I47" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A48" s="9" t="s">
-        <v>30</v>
+      <c r="A48" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="B48" s="1">
         <v>47398000</v>
       </c>
       <c r="C48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A49" s="9" t="s">
-        <v>30</v>
+      <c r="A49" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="B49" s="1">
         <v>53360000</v>
       </c>
       <c r="D49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A50" s="9" t="s">
-        <v>30</v>
+      <c r="A50" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="B50" s="1">
         <v>79019000</v>
       </c>
       <c r="E50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H50" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50" t="s">
         <v>19</v>
-      </c>
-      <c r="I50" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1553,7 +1559,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -1569,1009 +1575,1009 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8"/>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.6">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="7" t="s">
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.6">
-      <c r="A2" s="6"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="6"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A3" s="3" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B3" s="5">
         <v>5366000</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A4" s="3" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B4" s="5">
         <v>6734000</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A5" s="3" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B5" s="5">
         <v>8025000</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A6" s="3" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B6" s="5">
         <v>12035000</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A7" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="5">
         <v>4787000</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="5">
         <v>6033000</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="5">
         <v>7282000</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="5">
         <v>11070000</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="5">
         <v>5835000</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="5">
         <v>7046000</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="5">
         <v>8372000</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="5">
         <v>13050000</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="5">
         <v>6713000</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A16" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="5">
         <v>8082000</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="5">
         <v>8687000</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A18" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="5">
         <v>13802000</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="5">
         <v>7610000</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="5">
         <v>9131000</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="5">
         <v>9647000</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A22" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="5">
         <v>16142000</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A23" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="5">
         <v>8837000</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="5">
         <v>10509000</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A25" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="5">
         <v>11293000</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A26" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="5">
         <v>18131000</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A27" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="5">
         <v>10377000</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A28" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="5">
         <v>12531000</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A29" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" s="5">
         <v>14712000</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A30" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B30" s="5">
         <v>22699000</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A31" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" s="5">
         <v>13073000</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A32" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="5">
         <v>16298000</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A33" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" s="5">
         <v>17410000</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A34" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B34" s="5">
         <v>26505000</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A35" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B35" s="5">
         <v>16197000</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A36" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B36" s="5">
         <v>19922000</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A37" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B37" s="5">
         <v>22485000</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A38" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B38" s="5">
         <v>33777000</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H38" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A39" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B39" s="5">
         <v>19214000</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A40" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B40" s="5">
         <v>24140000</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A41" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B41" s="5">
         <v>29218000</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A42" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B42" s="5">
         <v>39629000</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H42" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A43" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B43" s="5">
         <v>21273000</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A44" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B44" s="5">
         <v>28238000</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A45" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B45" s="5">
         <v>32323000</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A46" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B46" s="5">
         <v>47420000</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H46" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I46" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A47" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B47" s="5">
         <v>28387000</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A48" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B48" s="5">
         <v>39639000</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A49" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B49" s="5">
         <v>46574000</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A50" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B50" s="5">
         <v>67559000</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H50" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2582,6 +2588,7 @@
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>